<commit_message>
update dopo colloquio con il prof
</commit_message>
<xml_diff>
--- a/01_Glossario.xlsx
+++ b/01_Glossario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Progetto-Laboratorio-BSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mansitos-Notebook\Documents\GitHub\Progetto-Laboratorio-BSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2EBE9C-1D49-4F08-AA73-94BAF4D5B3D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F788C6F8-4E79-4883-B9CE-E28498CDE1AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="750" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="90">
   <si>
     <t>Termine</t>
   </si>
@@ -247,6 +247,60 @@
   </si>
   <si>
     <t>Mette in relazione un addetto delle pulizie con le abitazioni che deve pulire.</t>
+  </si>
+  <si>
+    <t>VERSIONE 4</t>
+  </si>
+  <si>
+    <t>veterinario, gabbia, genere</t>
+  </si>
+  <si>
+    <t>È formata da un insieme di abitazioni in essa collocate.</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>collocata</t>
+  </si>
+  <si>
+    <t>Le gabbie sono situate in un'abitazione.</t>
+  </si>
+  <si>
+    <t>genere</t>
+  </si>
+  <si>
+    <t>gabbia, addetto pulizie, area, genere</t>
+  </si>
+  <si>
+    <t>assegnato</t>
+  </si>
+  <si>
+    <t>abitazione, esemplare</t>
+  </si>
+  <si>
+    <t>Identifica il genere di un esemplare con cui è in relazione. Identifica il genere di animali che possono essere contenuti nelle gabbie di una determinata abitazione.</t>
+  </si>
+  <si>
+    <t>Mette in relazione una abitazione con un genere per identificare il genere di animali che possono essere contenuti nelle sue gabbie.</t>
+  </si>
+  <si>
+    <t>abitazione, genere</t>
+  </si>
+  <si>
+    <t>esemplare, genere</t>
+  </si>
+  <si>
+    <t>Mette in relazione un esemplare con un genere per identificarne l'appartenenza.</t>
+  </si>
+  <si>
+    <t>È identificato da un codice univoco all'interno del genere di appartenenza.</t>
+  </si>
+  <si>
+    <t>È destinata ad un determinato genere di animali; ogni abitazione contiene un insieme di gabbie; ogni abitazione ha un addetto che pulisce ciascuna gabbia.</t>
+  </si>
+  <si>
+    <t>Mette in relazione un'abitazione con una determinata area.</t>
   </si>
 </sst>
 </file>
@@ -466,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -552,6 +606,48 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -834,29 +930,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R21"/>
+  <dimension ref="B2:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="P14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="6" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" customWidth="1"/>
-    <col min="11" max="12" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" customWidth="1"/>
-    <col min="15" max="15" width="24.7109375" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" customWidth="1"/>
-    <col min="17" max="18" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="6" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1"/>
+    <col min="11" max="12" width="17.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="15" max="15" width="24.6640625" customWidth="1"/>
+    <col min="16" max="16" width="17.88671875" customWidth="1"/>
+    <col min="17" max="18" width="17.6640625" customWidth="1"/>
+    <col min="20" max="20" width="17.6640625" customWidth="1"/>
+    <col min="21" max="21" width="24.6640625" customWidth="1"/>
+    <col min="22" max="22" width="17.88671875" customWidth="1"/>
+    <col min="23" max="24" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>42</v>
       </c>
@@ -866,8 +966,11 @@
       <c r="N2" s="26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T2" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -913,8 +1016,23 @@
       <c r="R3" s="16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
@@ -960,8 +1078,23 @@
       <c r="R4" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="T4" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>68</v>
       </c>
@@ -1007,8 +1140,23 @@
       <c r="R5" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="T5" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="U5" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="V5" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="W5" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="X5" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1054,8 +1202,23 @@
       <c r="R6" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="T6" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="U6" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="V6" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="W6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="X6" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
@@ -1101,8 +1264,23 @@
       <c r="R7" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="T7" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="U7" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="V7" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="W7" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="X7" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="18"/>
       <c r="D8" s="9"/>
@@ -1134,8 +1312,21 @@
       <c r="R8" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" s="2" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T8" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="U8" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="V8" s="38"/>
+      <c r="W8" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="X8" s="38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" s="2" customFormat="1" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>37</v>
       </c>
@@ -1175,8 +1366,21 @@
       <c r="R9" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="T9" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="U9" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="V9" s="38"/>
+      <c r="W9" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="X9" s="38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>36</v>
       </c>
@@ -1216,8 +1420,21 @@
       <c r="R10" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="T10" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="U10" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="V10" s="38"/>
+      <c r="W10" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="X10" s="38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
@@ -1257,8 +1474,21 @@
       <c r="R11" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="T11" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="V11" s="38"/>
+      <c r="W11" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="X11" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
@@ -1300,8 +1530,23 @@
       <c r="R12" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="T12" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="U12" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="V12" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="W12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="X12" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>32</v>
       </c>
@@ -1341,8 +1586,21 @@
       <c r="R13" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="2:18" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="T13" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="U13" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="V13" s="39"/>
+      <c r="W13" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="X13" s="38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1382,8 +1640,21 @@
       <c r="R14" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T14" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="U14" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="V14" s="38"/>
+      <c r="W14" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="X14" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7" t="s">
         <v>35</v>
       </c>
@@ -1429,8 +1700,23 @@
       <c r="R15" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T15" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="U15" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="V15" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="W15" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="X15" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1446,8 +1732,21 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T16" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="U16" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="V16" s="44"/>
+      <c r="W16" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="X16" s="44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1463,8 +1762,21 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T17" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="U17" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="V17" s="44"/>
+      <c r="W17" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="X17" s="44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1480,8 +1792,21 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T18" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="U18" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="V18" s="44"/>
+      <c r="W18" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="X18" s="44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1497,8 +1822,13 @@
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T19" s="3"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1514,11 +1844,17 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T20" s="3"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="H21" s="4"/>
       <c r="N21" s="4"/>
+      <c r="T21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2 del day
</commit_message>
<xml_diff>
--- a/01_Glossario.xlsx
+++ b/01_Glossario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mansitos-Notebook\Documents\GitHub\Progetto-Laboratorio-BSD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF9153-356B-4ECE-BFC9-1804891B3AFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121CE731-350E-4A76-851C-F7C41DE62930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6552" yWindow="-288" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6132" yWindow="6504" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,9 +288,6 @@
     <t>Mette in relazione un esemplare con un genere per identificarne l'appartenenza.</t>
   </si>
   <si>
-    <t>È identificato da un codice univoco all'interno del genere di appartenenza.</t>
-  </si>
-  <si>
     <t>È destinata ad un determinato genere di animali; ogni abitazione contiene un insieme di gabbie; ogni abitazione ha un addetto che pulisce ciascuna gabbia.</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>tipo</t>
+  </si>
+  <si>
+    <t>È dal suo genere e da un codice unico all'interno del genere di appartenenza.</t>
   </si>
 </sst>
 </file>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1180,7 +1180,7 @@
         <v>68</v>
       </c>
       <c r="U5" s="25" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="V5" s="38" t="s">
         <v>5</v>
@@ -1304,7 +1304,7 @@
         <v>12</v>
       </c>
       <c r="U7" s="37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="V7" s="38" t="s">
         <v>9</v>
@@ -1352,7 +1352,7 @@
         <v>76</v>
       </c>
       <c r="U8" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="V8" s="38"/>
       <c r="W8" s="29" t="s">
@@ -1406,7 +1406,7 @@
         <v>75</v>
       </c>
       <c r="U9" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V9" s="38"/>
       <c r="W9" s="29" t="s">
@@ -1460,7 +1460,7 @@
         <v>54</v>
       </c>
       <c r="U10" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V10" s="38"/>
       <c r="W10" s="29" t="s">
@@ -1514,7 +1514,7 @@
         <v>10</v>
       </c>
       <c r="U11" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V11" s="38"/>
       <c r="W11" s="29" t="s">
@@ -1570,7 +1570,7 @@
         <v>18</v>
       </c>
       <c r="U12" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="V12" s="38" t="s">
         <v>17</v>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="V13" s="39"/>
       <c r="W13" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X13" s="38" t="s">
         <v>23</v>
@@ -1740,7 +1740,7 @@
         <v>49</v>
       </c>
       <c r="U15" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="V15" s="41" t="s">
         <v>30</v>
@@ -1775,7 +1775,7 @@
         <v>81</v>
       </c>
       <c r="V16" s="44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W16" s="30" t="s">
         <v>80</v>
@@ -1804,7 +1804,7 @@
         <v>79</v>
       </c>
       <c r="U17" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V17" s="44"/>
       <c r="W17" s="30" t="s">

</xml_diff>

<commit_message>
Bozza relazione + stile consistent tra file
</commit_message>
<xml_diff>
--- a/01_Glossario.xlsx
+++ b/01_Glossario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mansitos-Notebook\Documents\GitHub\Progetto-Laboratorio-BSD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danyp\Documents\Programmazione\Basi di Dati - Progetto Gestione Zoo\Progetto-Laboratorio-BSD\old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121CE731-350E-4A76-851C-F7C41DE62930}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329EA806-9B7F-48E3-BE63-E3E5EE193B9E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6132" yWindow="6504" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="97">
   <si>
     <t>Termine</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>È dal suo genere e da un codice unico all'interno del genere di appartenenza.</t>
+  </si>
+  <si>
+    <t>VERSIONE 4 (con grigio header corretto)</t>
   </si>
 </sst>
 </file>
@@ -357,7 +360,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,6 +391,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -552,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -684,6 +699,60 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -692,6 +761,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFBFBFBF"/>
+      <color rgb="FFF8F8FF"/>
+      <color rgb="FFFFFDD0"/>
+      <color rgb="FFF8F8F8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -966,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:X21"/>
+  <dimension ref="B2:AD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,9 +1067,13 @@
     <col min="21" max="21" width="24.6640625" customWidth="1"/>
     <col min="22" max="22" width="17.88671875" customWidth="1"/>
     <col min="23" max="24" width="17.6640625" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" customWidth="1"/>
+    <col min="27" max="27" width="24.6640625" customWidth="1"/>
+    <col min="28" max="28" width="17.88671875" customWidth="1"/>
+    <col min="29" max="30" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>42</v>
       </c>
@@ -1003,10 +1084,13 @@
         <v>50</v>
       </c>
       <c r="T2" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z2" s="26" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="2:24" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:30" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -1052,23 +1136,38 @@
       <c r="R3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="T3" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="U3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="V3" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="17" t="s">
+      <c r="W3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="62" t="s">
         <v>4</v>
       </c>
+      <c r="Z3" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="62" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="2:24" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
@@ -1129,8 +1228,23 @@
       <c r="X4" s="35" t="s">
         <v>27</v>
       </c>
+      <c r="Z4" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA4" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB4" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC4" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD4" s="50" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="2:24" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:30" s="2" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>68</v>
       </c>
@@ -1191,8 +1305,23 @@
       <c r="X5" s="38" t="s">
         <v>6</v>
       </c>
+      <c r="Z5" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA5" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB5" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC5" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD5" s="53" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="2:24" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:30" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1253,8 +1382,23 @@
       <c r="X6" s="38" t="s">
         <v>6</v>
       </c>
+      <c r="Z6" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA6" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB6" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC6" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD6" s="53" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="7" spans="2:24" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:30" s="2" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
@@ -1315,8 +1459,23 @@
       <c r="X7" s="38" t="s">
         <v>6</v>
       </c>
+      <c r="Z7" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA7" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB7" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC7" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD7" s="53" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="2:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:30" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
       <c r="C8" s="18"/>
       <c r="D8" s="9"/>
@@ -1361,8 +1520,21 @@
       <c r="X8" s="38" t="s">
         <v>23</v>
       </c>
+      <c r="Z8" s="51" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA8" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB8" s="53"/>
+      <c r="AC8" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD8" s="53" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="9" spans="2:24" s="2" customFormat="1" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:30" s="2" customFormat="1" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>37</v>
       </c>
@@ -1415,8 +1587,21 @@
       <c r="X9" s="38" t="s">
         <v>23</v>
       </c>
+      <c r="Z9" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA9" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB9" s="53"/>
+      <c r="AC9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="53" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="10" spans="2:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:30" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>36</v>
       </c>
@@ -1469,8 +1654,21 @@
       <c r="X10" s="38" t="s">
         <v>23</v>
       </c>
+      <c r="Z10" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA10" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB10" s="53"/>
+      <c r="AC10" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD10" s="53" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="11" spans="2:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:30" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
@@ -1523,8 +1721,21 @@
       <c r="X11" s="38" t="s">
         <v>6</v>
       </c>
+      <c r="Z11" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB11" s="53"/>
+      <c r="AC11" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD11" s="53" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="12" spans="2:24" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:30" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
@@ -1581,8 +1792,23 @@
       <c r="X12" s="38" t="s">
         <v>6</v>
       </c>
+      <c r="Z12" s="51" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA12" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB12" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC12" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD12" s="53" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="13" spans="2:24" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:30" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>32</v>
       </c>
@@ -1635,8 +1861,21 @@
       <c r="X13" s="38" t="s">
         <v>23</v>
       </c>
+      <c r="Z13" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA13" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB13" s="56"/>
+      <c r="AC13" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD13" s="53" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="14" spans="2:24" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:30" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1689,8 +1928,21 @@
       <c r="X14" s="38" t="s">
         <v>6</v>
       </c>
+      <c r="Z14" s="51" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA14" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB14" s="53"/>
+      <c r="AC14" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD14" s="53" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="15" spans="2:24" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:30" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7" t="s">
         <v>35</v>
       </c>
@@ -1751,8 +2003,23 @@
       <c r="X15" s="41" t="s">
         <v>23</v>
       </c>
+      <c r="Z15" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA15" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB15" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC15" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD15" s="59" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="16" spans="2:24" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:30" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1783,8 +2050,23 @@
       <c r="X16" s="44" t="s">
         <v>6</v>
       </c>
+      <c r="Z16" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA16" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB16" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC16" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD16" s="59" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="17" spans="2:24" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:30" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1813,8 +2095,21 @@
       <c r="X17" s="44" t="s">
         <v>23</v>
       </c>
+      <c r="Z17" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA17" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB17" s="59"/>
+      <c r="AC17" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD17" s="59" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="18" spans="2:24" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:30" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1843,8 +2138,21 @@
       <c r="X18" s="44" t="s">
         <v>23</v>
       </c>
+      <c r="Z18" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA18" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB18" s="59"/>
+      <c r="AC18" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD18" s="59" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1865,8 +2173,13 @@
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1887,12 +2200,18 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="H21" s="4"/>
       <c r="N21" s="4"/>
       <c r="T21" s="4"/>
+      <c r="Z21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>